<commit_message>
Adicionado Setores e Atualizações 24-01
</commit_message>
<xml_diff>
--- a/diretoria-vouchers.xlsx
+++ b/diretoria-vouchers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,16 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Retirado Por</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Data Retirada</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +466,8 @@
           <t>Usado</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +480,8 @@
           <t>Usado</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -480,6 +494,16 @@
           <t>Usado</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lucas Almeida (CPF: 28266996873)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-01-24 15:56:03</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -492,6 +516,16 @@
           <t>Usado</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Lucas Almeida (CPF: 28266996873)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-01-24 15:56:03</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -504,6 +538,16 @@
           <t>Usado</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Lucas Almeida (CPF: 28266996873)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-01-24 16:22:03</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -516,6 +560,16 @@
           <t>Usado</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Lucas Almeida (CPF: 28266996873)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-01-24 17:12:57</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -525,9 +579,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -537,9 +593,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -549,9 +607,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -561,9 +621,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -573,9 +635,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -585,9 +649,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -597,9 +663,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -609,9 +677,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -621,9 +691,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -633,9 +705,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -645,9 +719,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Usado</t>
-        </is>
-      </c>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -660,6 +736,8 @@
           <t>Disponível</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -672,6 +750,8 @@
           <t>Disponível</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -684,6 +764,8 @@
           <t>Disponível</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -696,6 +778,8 @@
           <t>Disponível</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>